<commit_message>
``` refactor(src/cli/argument_parser.py, frozen_dist/zr_daily_report/src/ui/filedialog_selector.py, frozen_dist/zr_daily_report/src/core/statement_handler.py): 优化代码逻辑和窗口调整功能
在 `src/cli/argument_parser.py` 中添加了新的日期格式示例。在 `frozen_dist/zr_daily_report/src/ui/filedialog_selector.py` 中：- 增加了初始等待时间，确保窗口完全初始化。- 扩展了窗口标题匹配列表，包括常见的中文和英文标题。- 增加了尝试次数，并优化了查找窗口的逻辑。
- 添加了对常见文件对话框类名的支持。
- 增加了日志记录，以便更好地调试和处理异常情况。

在 `frozen_dist/zr_daily_report/src/core/statement_handler.py` 中：- 修改了合并单元格的范围。
- 优化了月份标题的写入方式，使其更加灵活。
- 在C5单元格合并区域写入年份，并在C6到N6单元格分别写入1月到12月。
- 更新了A22单元格中的日期格式，增加了制单人信息。
```
</commit_message>
<xml_diff>
--- a/frozen_dist/zr_daily_report/template/statement_template.xlsx
+++ b/frozen_dist/zr_daily_report/template/statement_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12255"/>
+    <workbookView windowWidth="27945" windowHeight="12255" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="中润对账单" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>客户名称：浙江巨跃齿轮有限公司</t>
   </si>
@@ -149,7 +149,7 @@
   </si>
   <si>
     <t xml:space="preserve">                          
-                          用油型号
+                        用油型号
 </t>
   </si>
   <si>
@@ -158,99 +158,6 @@
   <si>
     <t>2025年
 7月</t>
-  </si>
-  <si>
-    <t>7.1</t>
-  </si>
-  <si>
-    <t>7.2</t>
-  </si>
-  <si>
-    <t>7.3</t>
-  </si>
-  <si>
-    <t>7.4</t>
-  </si>
-  <si>
-    <t>7.5</t>
-  </si>
-  <si>
-    <t>7.6</t>
-  </si>
-  <si>
-    <t>7.7</t>
-  </si>
-  <si>
-    <t>7.8</t>
-  </si>
-  <si>
-    <t>7.9</t>
-  </si>
-  <si>
-    <t>7.10</t>
-  </si>
-  <si>
-    <t>7.11</t>
-  </si>
-  <si>
-    <t>7.12</t>
-  </si>
-  <si>
-    <t>7.13</t>
-  </si>
-  <si>
-    <t>7.14</t>
-  </si>
-  <si>
-    <t>7.15</t>
-  </si>
-  <si>
-    <t>7.16</t>
-  </si>
-  <si>
-    <t>7.17</t>
-  </si>
-  <si>
-    <t>7.18</t>
-  </si>
-  <si>
-    <t>7.19</t>
-  </si>
-  <si>
-    <t>7.20</t>
-  </si>
-  <si>
-    <t>7.21</t>
-  </si>
-  <si>
-    <t>7.22</t>
-  </si>
-  <si>
-    <t>7.23</t>
-  </si>
-  <si>
-    <t>7.24</t>
-  </si>
-  <si>
-    <t>7.25</t>
-  </si>
-  <si>
-    <t>7.26</t>
-  </si>
-  <si>
-    <t>7.27</t>
-  </si>
-  <si>
-    <t>7.28</t>
-  </si>
-  <si>
-    <t>7.29</t>
-  </si>
-  <si>
-    <t>7.30</t>
-  </si>
-  <si>
-    <t>7.31</t>
   </si>
   <si>
     <t>合计</t>
@@ -263,14 +170,31 @@
 </t>
   </si>
   <si>
-    <t>2025年</t>
+    <t>2024年</t>
   </si>
   <si>
-    <t xml:space="preserve">
-设备编号</t>
+    <t>设备编号</t>
   </si>
   <si>
-    <t>月  份</t>
+    <t>油品名称</t>
+  </si>
+  <si>
+    <t>1月</t>
+  </si>
+  <si>
+    <t>2月</t>
+  </si>
+  <si>
+    <t>3月</t>
+  </si>
+  <si>
+    <t>4月</t>
+  </si>
+  <si>
+    <t>5月</t>
+  </si>
+  <si>
+    <t>6月</t>
   </si>
   <si>
     <t>7月</t>
@@ -302,15 +226,15 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0_);[Red]\(0.0\)"/>
     <numFmt numFmtId="177" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="178" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
-    <numFmt numFmtId="179" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="180" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
-    <numFmt numFmtId="181" formatCode="0.00_ "/>
-    <numFmt numFmtId="182" formatCode="General&quot;月&quot;"/>
+    <numFmt numFmtId="178" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="179" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="180" formatCode="0.00_ "/>
+    <numFmt numFmtId="181" formatCode="General&quot;月&quot;"/>
+    <numFmt numFmtId="182" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
     <numFmt numFmtId="183" formatCode="0_ "/>
     <numFmt numFmtId="184" formatCode="[DBNum2][$RMB]General;[Red][DBNum2][$RMB]General"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="38">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,32 +283,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="微软雅黑"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="9" tint="-0.25"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="微软雅黑"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="0"/>
-      <name val="微软雅黑"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
@@ -841,7 +739,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -865,61 +763,11 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.15"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0" tint="-0.15"/>
       </left>
       <right style="thin">
         <color theme="0" tint="-0.15"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
       </right>
       <top style="thin">
         <color theme="0" tint="-0.14996795556505"/>
@@ -946,48 +794,57 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFCADFB3"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFCADFB3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCADFB3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFCADFB3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCADFB3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCADFB3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCADFB3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCADFB3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.15"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color theme="0" tint="-0.14996795556505"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </right>
-      <top/>
+      </top>
       <bottom style="thin">
         <color theme="0" tint="-0.14996795556505"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.149937437055574"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.149937437055574"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.149937437055574"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="0" tint="-0.14996795556505"/>
       </top>
@@ -998,7 +855,7 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.15"/>
+        <color theme="0" tint="-0.14996795556505"/>
       </left>
       <right/>
       <top style="thin">
@@ -1066,19 +923,6 @@
         <color theme="0"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCADFB3"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFCADFB3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCADFB3"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1349,137 +1193,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="11" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="12" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1498,9 +1342,6 @@
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1510,367 +1351,310 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="4" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="8" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="8" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="8" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="7" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="8" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="8" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="11" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="8" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="8" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="12" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="12" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="12" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="183" fontId="12" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="12" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="14" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="14" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="15" fillId="8" borderId="16" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="16" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="14" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="14" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="18" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="18" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="19" fillId="8" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="20" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="18" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="18" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2058,105 +1842,13 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>每日用量明细!$B$6:$B$36</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>@</c:formatCode>
                 <c:ptCount val="31"/>
-                <c:pt idx="0" c:formatCode="@">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="1" c:formatCode="@">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="2" c:formatCode="@">
-                  <c:v>7.3</c:v>
-                </c:pt>
-                <c:pt idx="3" c:formatCode="@">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="4" c:formatCode="@">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="5" c:formatCode="@">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="6" c:formatCode="@">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="7" c:formatCode="@">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="8" c:formatCode="@">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="9" c:formatCode="@">
-                  <c:v>7.10</c:v>
-                </c:pt>
-                <c:pt idx="10" c:formatCode="@">
-                  <c:v>7.11</c:v>
-                </c:pt>
-                <c:pt idx="11" c:formatCode="@">
-                  <c:v>7.12</c:v>
-                </c:pt>
-                <c:pt idx="12" c:formatCode="@">
-                  <c:v>7.13</c:v>
-                </c:pt>
-                <c:pt idx="13" c:formatCode="@">
-                  <c:v>7.14</c:v>
-                </c:pt>
-                <c:pt idx="14" c:formatCode="@">
-                  <c:v>7.15</c:v>
-                </c:pt>
-                <c:pt idx="15" c:formatCode="@">
-                  <c:v>7.16</c:v>
-                </c:pt>
-                <c:pt idx="16" c:formatCode="@">
-                  <c:v>7.17</c:v>
-                </c:pt>
-                <c:pt idx="17" c:formatCode="@">
-                  <c:v>7.18</c:v>
-                </c:pt>
-                <c:pt idx="18" c:formatCode="@">
-                  <c:v>7.19</c:v>
-                </c:pt>
-                <c:pt idx="19" c:formatCode="@">
-                  <c:v>7.20</c:v>
-                </c:pt>
-                <c:pt idx="20" c:formatCode="@">
-                  <c:v>7.21</c:v>
-                </c:pt>
-                <c:pt idx="21" c:formatCode="@">
-                  <c:v>7.22</c:v>
-                </c:pt>
-                <c:pt idx="22" c:formatCode="@">
-                  <c:v>7.23</c:v>
-                </c:pt>
-                <c:pt idx="23" c:formatCode="@">
-                  <c:v>7.24</c:v>
-                </c:pt>
-                <c:pt idx="24" c:formatCode="@">
-                  <c:v>7.25</c:v>
-                </c:pt>
-                <c:pt idx="25" c:formatCode="@">
-                  <c:v>7.26</c:v>
-                </c:pt>
-                <c:pt idx="26" c:formatCode="@">
-                  <c:v>7.27</c:v>
-                </c:pt>
-                <c:pt idx="27" c:formatCode="@">
-                  <c:v>7.28</c:v>
-                </c:pt>
-                <c:pt idx="28" c:formatCode="@">
-                  <c:v>7.29</c:v>
-                </c:pt>
-                <c:pt idx="29" c:formatCode="@">
-                  <c:v>7.30</c:v>
-                </c:pt>
-                <c:pt idx="30" c:formatCode="@">
-                  <c:v>7.31</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2164,99 +1856,6 @@
               <c:numCache>
                 <c:formatCode>@</c:formatCode>
                 <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2271,7 +1870,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>全合成研磨切削液S8L-1</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2292,105 +1891,13 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>每日用量明细!$B$6:$B$36</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>@</c:formatCode>
                 <c:ptCount val="31"/>
-                <c:pt idx="0" c:formatCode="@">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="1" c:formatCode="@">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="2" c:formatCode="@">
-                  <c:v>7.3</c:v>
-                </c:pt>
-                <c:pt idx="3" c:formatCode="@">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="4" c:formatCode="@">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="5" c:formatCode="@">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="6" c:formatCode="@">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="7" c:formatCode="@">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="8" c:formatCode="@">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="9" c:formatCode="@">
-                  <c:v>7.10</c:v>
-                </c:pt>
-                <c:pt idx="10" c:formatCode="@">
-                  <c:v>7.11</c:v>
-                </c:pt>
-                <c:pt idx="11" c:formatCode="@">
-                  <c:v>7.12</c:v>
-                </c:pt>
-                <c:pt idx="12" c:formatCode="@">
-                  <c:v>7.13</c:v>
-                </c:pt>
-                <c:pt idx="13" c:formatCode="@">
-                  <c:v>7.14</c:v>
-                </c:pt>
-                <c:pt idx="14" c:formatCode="@">
-                  <c:v>7.15</c:v>
-                </c:pt>
-                <c:pt idx="15" c:formatCode="@">
-                  <c:v>7.16</c:v>
-                </c:pt>
-                <c:pt idx="16" c:formatCode="@">
-                  <c:v>7.17</c:v>
-                </c:pt>
-                <c:pt idx="17" c:formatCode="@">
-                  <c:v>7.18</c:v>
-                </c:pt>
-                <c:pt idx="18" c:formatCode="@">
-                  <c:v>7.19</c:v>
-                </c:pt>
-                <c:pt idx="19" c:formatCode="@">
-                  <c:v>7.20</c:v>
-                </c:pt>
-                <c:pt idx="20" c:formatCode="@">
-                  <c:v>7.21</c:v>
-                </c:pt>
-                <c:pt idx="21" c:formatCode="@">
-                  <c:v>7.22</c:v>
-                </c:pt>
-                <c:pt idx="22" c:formatCode="@">
-                  <c:v>7.23</c:v>
-                </c:pt>
-                <c:pt idx="23" c:formatCode="@">
-                  <c:v>7.24</c:v>
-                </c:pt>
-                <c:pt idx="24" c:formatCode="@">
-                  <c:v>7.25</c:v>
-                </c:pt>
-                <c:pt idx="25" c:formatCode="@">
-                  <c:v>7.26</c:v>
-                </c:pt>
-                <c:pt idx="26" c:formatCode="@">
-                  <c:v>7.27</c:v>
-                </c:pt>
-                <c:pt idx="27" c:formatCode="@">
-                  <c:v>7.28</c:v>
-                </c:pt>
-                <c:pt idx="28" c:formatCode="@">
-                  <c:v>7.29</c:v>
-                </c:pt>
-                <c:pt idx="29" c:formatCode="@">
-                  <c:v>7.30</c:v>
-                </c:pt>
-                <c:pt idx="30" c:formatCode="@">
-                  <c:v>7.31</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2412,7 +1919,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>全合成研磨切削液825-1</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2433,105 +1940,13 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>每日用量明细!$B$6:$B$36</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>@</c:formatCode>
                 <c:ptCount val="31"/>
-                <c:pt idx="0" c:formatCode="@">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="1" c:formatCode="@">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="2" c:formatCode="@">
-                  <c:v>7.3</c:v>
-                </c:pt>
-                <c:pt idx="3" c:formatCode="@">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="4" c:formatCode="@">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="5" c:formatCode="@">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="6" c:formatCode="@">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="7" c:formatCode="@">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="8" c:formatCode="@">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="9" c:formatCode="@">
-                  <c:v>7.10</c:v>
-                </c:pt>
-                <c:pt idx="10" c:formatCode="@">
-                  <c:v>7.11</c:v>
-                </c:pt>
-                <c:pt idx="11" c:formatCode="@">
-                  <c:v>7.12</c:v>
-                </c:pt>
-                <c:pt idx="12" c:formatCode="@">
-                  <c:v>7.13</c:v>
-                </c:pt>
-                <c:pt idx="13" c:formatCode="@">
-                  <c:v>7.14</c:v>
-                </c:pt>
-                <c:pt idx="14" c:formatCode="@">
-                  <c:v>7.15</c:v>
-                </c:pt>
-                <c:pt idx="15" c:formatCode="@">
-                  <c:v>7.16</c:v>
-                </c:pt>
-                <c:pt idx="16" c:formatCode="@">
-                  <c:v>7.17</c:v>
-                </c:pt>
-                <c:pt idx="17" c:formatCode="@">
-                  <c:v>7.18</c:v>
-                </c:pt>
-                <c:pt idx="18" c:formatCode="@">
-                  <c:v>7.19</c:v>
-                </c:pt>
-                <c:pt idx="19" c:formatCode="@">
-                  <c:v>7.20</c:v>
-                </c:pt>
-                <c:pt idx="20" c:formatCode="@">
-                  <c:v>7.21</c:v>
-                </c:pt>
-                <c:pt idx="21" c:formatCode="@">
-                  <c:v>7.22</c:v>
-                </c:pt>
-                <c:pt idx="22" c:formatCode="@">
-                  <c:v>7.23</c:v>
-                </c:pt>
-                <c:pt idx="23" c:formatCode="@">
-                  <c:v>7.24</c:v>
-                </c:pt>
-                <c:pt idx="24" c:formatCode="@">
-                  <c:v>7.25</c:v>
-                </c:pt>
-                <c:pt idx="25" c:formatCode="@">
-                  <c:v>7.26</c:v>
-                </c:pt>
-                <c:pt idx="26" c:formatCode="@">
-                  <c:v>7.27</c:v>
-                </c:pt>
-                <c:pt idx="27" c:formatCode="@">
-                  <c:v>7.28</c:v>
-                </c:pt>
-                <c:pt idx="28" c:formatCode="@">
-                  <c:v>7.29</c:v>
-                </c:pt>
-                <c:pt idx="29" c:formatCode="@">
-                  <c:v>7.30</c:v>
-                </c:pt>
-                <c:pt idx="30" c:formatCode="@">
-                  <c:v>7.31</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2553,7 +1968,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>全合成研磨切削液S8L-2</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2574,105 +1989,13 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>每日用量明细!$B$6:$B$36</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>@</c:formatCode>
                 <c:ptCount val="31"/>
-                <c:pt idx="0" c:formatCode="@">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="1" c:formatCode="@">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="2" c:formatCode="@">
-                  <c:v>7.3</c:v>
-                </c:pt>
-                <c:pt idx="3" c:formatCode="@">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="4" c:formatCode="@">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="5" c:formatCode="@">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="6" c:formatCode="@">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="7" c:formatCode="@">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="8" c:formatCode="@">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="9" c:formatCode="@">
-                  <c:v>7.10</c:v>
-                </c:pt>
-                <c:pt idx="10" c:formatCode="@">
-                  <c:v>7.11</c:v>
-                </c:pt>
-                <c:pt idx="11" c:formatCode="@">
-                  <c:v>7.12</c:v>
-                </c:pt>
-                <c:pt idx="12" c:formatCode="@">
-                  <c:v>7.13</c:v>
-                </c:pt>
-                <c:pt idx="13" c:formatCode="@">
-                  <c:v>7.14</c:v>
-                </c:pt>
-                <c:pt idx="14" c:formatCode="@">
-                  <c:v>7.15</c:v>
-                </c:pt>
-                <c:pt idx="15" c:formatCode="@">
-                  <c:v>7.16</c:v>
-                </c:pt>
-                <c:pt idx="16" c:formatCode="@">
-                  <c:v>7.17</c:v>
-                </c:pt>
-                <c:pt idx="17" c:formatCode="@">
-                  <c:v>7.18</c:v>
-                </c:pt>
-                <c:pt idx="18" c:formatCode="@">
-                  <c:v>7.19</c:v>
-                </c:pt>
-                <c:pt idx="19" c:formatCode="@">
-                  <c:v>7.20</c:v>
-                </c:pt>
-                <c:pt idx="20" c:formatCode="@">
-                  <c:v>7.21</c:v>
-                </c:pt>
-                <c:pt idx="21" c:formatCode="@">
-                  <c:v>7.22</c:v>
-                </c:pt>
-                <c:pt idx="22" c:formatCode="@">
-                  <c:v>7.23</c:v>
-                </c:pt>
-                <c:pt idx="23" c:formatCode="@">
-                  <c:v>7.24</c:v>
-                </c:pt>
-                <c:pt idx="24" c:formatCode="@">
-                  <c:v>7.25</c:v>
-                </c:pt>
-                <c:pt idx="25" c:formatCode="@">
-                  <c:v>7.26</c:v>
-                </c:pt>
-                <c:pt idx="26" c:formatCode="@">
-                  <c:v>7.27</c:v>
-                </c:pt>
-                <c:pt idx="27" c:formatCode="@">
-                  <c:v>7.28</c:v>
-                </c:pt>
-                <c:pt idx="28" c:formatCode="@">
-                  <c:v>7.29</c:v>
-                </c:pt>
-                <c:pt idx="29" c:formatCode="@">
-                  <c:v>7.30</c:v>
-                </c:pt>
-                <c:pt idx="30" c:formatCode="@">
-                  <c:v>7.31</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2694,7 +2017,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>全合成研磨切削液825-2</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2715,105 +2038,13 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>每日用量明细!$B$6:$B$36</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>@</c:formatCode>
                 <c:ptCount val="31"/>
-                <c:pt idx="0" c:formatCode="@">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="1" c:formatCode="@">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="2" c:formatCode="@">
-                  <c:v>7.3</c:v>
-                </c:pt>
-                <c:pt idx="3" c:formatCode="@">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="4" c:formatCode="@">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="5" c:formatCode="@">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="6" c:formatCode="@">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="7" c:formatCode="@">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="8" c:formatCode="@">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="9" c:formatCode="@">
-                  <c:v>7.10</c:v>
-                </c:pt>
-                <c:pt idx="10" c:formatCode="@">
-                  <c:v>7.11</c:v>
-                </c:pt>
-                <c:pt idx="11" c:formatCode="@">
-                  <c:v>7.12</c:v>
-                </c:pt>
-                <c:pt idx="12" c:formatCode="@">
-                  <c:v>7.13</c:v>
-                </c:pt>
-                <c:pt idx="13" c:formatCode="@">
-                  <c:v>7.14</c:v>
-                </c:pt>
-                <c:pt idx="14" c:formatCode="@">
-                  <c:v>7.15</c:v>
-                </c:pt>
-                <c:pt idx="15" c:formatCode="@">
-                  <c:v>7.16</c:v>
-                </c:pt>
-                <c:pt idx="16" c:formatCode="@">
-                  <c:v>7.17</c:v>
-                </c:pt>
-                <c:pt idx="17" c:formatCode="@">
-                  <c:v>7.18</c:v>
-                </c:pt>
-                <c:pt idx="18" c:formatCode="@">
-                  <c:v>7.19</c:v>
-                </c:pt>
-                <c:pt idx="19" c:formatCode="@">
-                  <c:v>7.20</c:v>
-                </c:pt>
-                <c:pt idx="20" c:formatCode="@">
-                  <c:v>7.21</c:v>
-                </c:pt>
-                <c:pt idx="21" c:formatCode="@">
-                  <c:v>7.22</c:v>
-                </c:pt>
-                <c:pt idx="22" c:formatCode="@">
-                  <c:v>7.23</c:v>
-                </c:pt>
-                <c:pt idx="23" c:formatCode="@">
-                  <c:v>7.24</c:v>
-                </c:pt>
-                <c:pt idx="24" c:formatCode="@">
-                  <c:v>7.25</c:v>
-                </c:pt>
-                <c:pt idx="25" c:formatCode="@">
-                  <c:v>7.26</c:v>
-                </c:pt>
-                <c:pt idx="26" c:formatCode="@">
-                  <c:v>7.27</c:v>
-                </c:pt>
-                <c:pt idx="27" c:formatCode="@">
-                  <c:v>7.28</c:v>
-                </c:pt>
-                <c:pt idx="28" c:formatCode="@">
-                  <c:v>7.29</c:v>
-                </c:pt>
-                <c:pt idx="29" c:formatCode="@">
-                  <c:v>7.30</c:v>
-                </c:pt>
-                <c:pt idx="30" c:formatCode="@">
-                  <c:v>7.31</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -3129,7 +2360,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7月</c:v>
+                  <c:v>1月</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3150,43 +2381,20 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>每月用量对比!$B$7:$B$11</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>全合成研磨切削液S8L-1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>全合成研磨切削液825-1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>全合成研磨切削液S8L-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>全合成研磨切削液825-2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>每月用量对比!$C$7:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00_ </c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>4190.26</c:v>
-                </c:pt>
-                <c:pt idx="1" c:formatCode="General">
-                  <c:v>10048.88</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43.25</c:v>
-                </c:pt>
-                <c:pt idx="3" c:formatCode="General">
-                  <c:v>190.21</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3200,7 +2408,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8月</c:v>
+                  <c:v>2月</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3221,30 +2429,19 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>每月用量对比!$B$7:$B$11</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>全合成研磨切削液S8L-1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>全合成研磨切削液825-1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>全合成研磨切削液S8L-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>全合成研磨切削液825-2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>每月用量对比!$D$7:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00_ </c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
@@ -3259,7 +2456,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9月</c:v>
+                  <c:v>3月</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3280,30 +2477,19 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>每月用量对比!$B$7:$B$11</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>全合成研磨切削液S8L-1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>全合成研磨切削液825-1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>全合成研磨切削液S8L-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>全合成研磨切削液825-2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>每月用量对比!$E$7:$E$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00_ </c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
@@ -3318,7 +2504,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10月</c:v>
+                  <c:v>4月</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3339,30 +2525,19 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>每月用量对比!$B$7:$B$11</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>全合成研磨切削液S8L-1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>全合成研磨切削液825-1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>全合成研磨切削液S8L-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>全合成研磨切削液825-2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>每月用量对比!$F$7:$F$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00_ </c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
@@ -3377,7 +2552,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>11月</c:v>
+                  <c:v>5月</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3398,30 +2573,19 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>每月用量对比!$B$7:$B$11</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>全合成研磨切削液S8L-1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>全合成研磨切削液825-1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>全合成研磨切削液S8L-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>全合成研磨切削液825-2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>每月用量对比!$G$7:$G$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00_ </c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
@@ -3436,7 +2600,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>12月</c:v>
+                  <c:v>6月</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3457,30 +2621,19 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>每月用量对比!$B$7:$B$11</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>全合成研磨切削液S8L-1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>全合成研磨切削液825-1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>全合成研磨切削液S8L-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>全合成研磨切削液825-2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>每月用量对比!$H$7:$H$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00_ </c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
@@ -3560,7 +2713,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00_ " sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3840,7 +2993,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MO24111301600017 全合成研磨切削液S8L-1</c:v>
+                  <c:v>设备编号 油品名称</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3859,47 +3012,55 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>每月用量对比!$C$5:$H$6</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>7月</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>8月</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>9月</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>10月</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>11月</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>12月</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2025年</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+            <c:strRef>
+              <c:f>每月用量对比!$C$6:$N$6</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1月</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2月</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3月</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4月</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5月</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6月</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7月</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8月</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9月</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10月</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11月</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12月</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>每月用量对比!$C$7:$H$7</c:f>
+              <c:f>(每月用量对比!$A$7:$N$7,每月用量对比!$C$7:$N$7)</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>4190.26</c:v>
-                </c:pt>
+                <c:ptCount val="26"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3907,17 +3068,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>每月用量对比!$A$8:$B$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MO25050803700013 全合成研磨切削液825-1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -3932,47 +3082,55 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>每月用量对比!$C$5:$H$6</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>7月</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>8月</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>9月</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>10月</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>11月</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>12月</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2025年</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+            <c:strRef>
+              <c:f>每月用量对比!$C$6:$N$6</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1月</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2月</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3月</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4月</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5月</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6月</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7月</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8月</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9月</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10月</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11月</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12月</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>每月用量对比!$C$8:$H$8</c:f>
+              <c:f>每月用量对比!$A$8:$N$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>10048.88</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="14"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3980,17 +3138,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>每月用量对比!$A$9:$B$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MO24082401300006 全合成研磨切削液S8L-2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent3"/>
@@ -4005,47 +3152,55 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>每月用量对比!$C$5:$H$6</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>7月</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>8月</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>9月</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>10月</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>11月</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>12月</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2025年</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+            <c:strRef>
+              <c:f>每月用量对比!$C$6:$N$6</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1月</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2月</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3月</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4月</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5月</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6月</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7月</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8月</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9月</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10月</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11月</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12月</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>每月用量对比!$C$9:$H$9</c:f>
+              <c:f>每月用量对比!$A$9:$N$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>43.25</c:v>
-                </c:pt>
+                <c:ptCount val="14"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4053,17 +3208,6 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>每月用量对比!$A$10:$B$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ZRPYA1AA0001 全合成研磨切削液825-2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent4"/>
@@ -4078,47 +3222,195 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>每月用量对比!$C$5:$H$6</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>7月</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>8月</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>9月</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>10月</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>11月</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>12月</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2025年</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+            <c:strRef>
+              <c:f>每月用量对比!$C$6:$N$6</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1月</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2月</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3月</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4月</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5月</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6月</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7月</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8月</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9月</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10月</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11月</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12月</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>每月用量对比!$C$10:$H$10</c:f>
+              <c:f>每月用量对比!$A$10:$N$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="14"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>每月用量对比!$C$6:$N$6</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>190.21</c:v>
-                </c:pt>
+                  <c:v>1月</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2月</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3月</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4月</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5月</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6月</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7月</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8月</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9月</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10月</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11月</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12月</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>每月用量对比!$A$11:$N$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="14"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>每月用量对比!$C$6:$N$6</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1月</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2月</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3月</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4月</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5月</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6月</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7月</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8月</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9月</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10月</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11月</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12月</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>每月用量对比!$A$12:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="14"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6474,7 +5766,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>624205</xdr:colOff>
+      <xdr:colOff>509905</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>216535</xdr:rowOff>
     </xdr:to>
@@ -6518,7 +5810,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>624205</xdr:colOff>
+      <xdr:colOff>509905</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>216535</xdr:rowOff>
     </xdr:to>
@@ -6604,16 +5896,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>14605</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>48260</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>5080</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6621,8 +5913,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1724025" y="4733925"/>
-        <a:ext cx="7653655" cy="2858135"/>
+        <a:off x="952500" y="5308600"/>
+        <a:ext cx="11720830" cy="3733800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7399,274 +6691,274 @@
   <sheetPr/>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="5.43333333333333" style="79" customWidth="1"/>
-    <col min="2" max="2" width="13.75" style="79" customWidth="1"/>
-    <col min="3" max="3" width="7.15833333333333" style="79" customWidth="1"/>
-    <col min="4" max="4" width="7.125" style="79" customWidth="1"/>
-    <col min="5" max="5" width="19" style="79" customWidth="1"/>
-    <col min="6" max="6" width="14.8333333333333" style="79" customWidth="1"/>
-    <col min="7" max="7" width="14.0416666666667" style="79" customWidth="1"/>
-    <col min="8" max="8" width="19.65" style="79" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="79"/>
-    <col min="10" max="11" width="9" style="79"/>
-    <col min="12" max="12" width="11.5" style="79"/>
-    <col min="13" max="16345" width="9" style="79"/>
+    <col min="1" max="1" width="5.43333333333333" style="59" customWidth="1"/>
+    <col min="2" max="2" width="13.75" style="59" customWidth="1"/>
+    <col min="3" max="3" width="7.15833333333333" style="59" customWidth="1"/>
+    <col min="4" max="4" width="7.125" style="59" customWidth="1"/>
+    <col min="5" max="5" width="19" style="59" customWidth="1"/>
+    <col min="6" max="6" width="14.8333333333333" style="59" customWidth="1"/>
+    <col min="7" max="7" width="14.0416666666667" style="59" customWidth="1"/>
+    <col min="8" max="8" width="19.65" style="59" customWidth="1"/>
+    <col min="9" max="9" width="11.5" style="59"/>
+    <col min="10" max="11" width="9" style="59"/>
+    <col min="12" max="12" width="11.5" style="59"/>
+    <col min="13" max="16345" width="9" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" s="79" customFormat="1" ht="7" customHeight="1"/>
-    <row r="2" s="79" customFormat="1" ht="21" customHeight="1" spans="4:5">
-      <c r="D2" s="81"/>
-      <c r="E2" s="82"/>
-    </row>
-    <row r="3" s="79" customFormat="1" ht="21" customHeight="1" spans="4:5">
-      <c r="D3" s="81"/>
-      <c r="E3" s="82"/>
-    </row>
-    <row r="4" s="79" customFormat="1" ht="5" customHeight="1"/>
-    <row r="5" s="79" customFormat="1" ht="21" customHeight="1" spans="1:8">
-      <c r="A5" s="83" t="s">
+    <row r="1" s="59" customFormat="1" ht="7" customHeight="1"/>
+    <row r="2" s="59" customFormat="1" ht="21" customHeight="1" spans="4:5">
+      <c r="D2" s="61"/>
+      <c r="E2" s="62"/>
+    </row>
+    <row r="3" s="59" customFormat="1" ht="21" customHeight="1" spans="4:5">
+      <c r="D3" s="61"/>
+      <c r="E3" s="62"/>
+    </row>
+    <row r="4" s="59" customFormat="1" ht="5" customHeight="1"/>
+    <row r="5" s="59" customFormat="1" ht="21" customHeight="1" spans="1:8">
+      <c r="A5" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="85" t="s">
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="86"/>
-    </row>
-    <row r="6" s="79" customFormat="1" ht="1" customHeight="1" spans="1:8">
-      <c r="A6" s="84"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-    </row>
-    <row r="7" s="79" customFormat="1" ht="2" customHeight="1"/>
-    <row r="8" s="79" customFormat="1" ht="30" customHeight="1" spans="1:8">
-      <c r="A8" s="87" t="s">
+      <c r="H5" s="66"/>
+    </row>
+    <row r="6" s="59" customFormat="1" ht="1" customHeight="1" spans="1:8">
+      <c r="A6" s="64"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+    </row>
+    <row r="7" s="59" customFormat="1" ht="2" customHeight="1"/>
+    <row r="8" s="59" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A8" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="87" t="s">
+      <c r="B8" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="87"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87" t="s">
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="88" t="s">
+      <c r="F8" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="89"/>
-      <c r="H8" s="87" t="s">
+      <c r="G8" s="69"/>
+      <c r="H8" s="67" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" s="80" customFormat="1" ht="25" customHeight="1" spans="1:9">
-      <c r="A9" s="90">
+    <row r="9" s="60" customFormat="1" ht="25" customHeight="1" spans="1:9">
+      <c r="A9" s="70">
         <v>1</v>
       </c>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="91"/>
-      <c r="D9" s="91"/>
-      <c r="E9" s="92" t="s">
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="93">
+      <c r="F9" s="73">
         <v>4190.26</v>
       </c>
-      <c r="G9" s="94"/>
-      <c r="H9" s="95"/>
-      <c r="I9" s="130"/>
-    </row>
-    <row r="10" s="79" customFormat="1" ht="25" customHeight="1" spans="1:8">
-      <c r="A10" s="96">
+      <c r="G9" s="74"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="110"/>
+    </row>
+    <row r="10" s="59" customFormat="1" ht="25" customHeight="1" spans="1:8">
+      <c r="A10" s="76">
         <v>2</v>
       </c>
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="97"/>
-      <c r="D10" s="97"/>
-      <c r="E10" s="97" t="s">
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="98">
+      <c r="F10" s="78">
         <v>10048.88</v>
       </c>
-      <c r="G10" s="99"/>
-      <c r="H10" s="100"/>
-    </row>
-    <row r="11" s="80" customFormat="1" ht="25" customHeight="1" spans="1:9">
-      <c r="A11" s="90">
+      <c r="G10" s="79"/>
+      <c r="H10" s="80"/>
+    </row>
+    <row r="11" s="60" customFormat="1" ht="25" customHeight="1" spans="1:9">
+      <c r="A11" s="70">
         <v>3</v>
       </c>
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="91"/>
-      <c r="D11" s="91"/>
-      <c r="E11" s="92" t="s">
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="93">
+      <c r="F11" s="73">
         <v>43.25</v>
       </c>
-      <c r="G11" s="94"/>
-      <c r="H11" s="101"/>
-      <c r="I11" s="130"/>
-    </row>
-    <row r="12" s="79" customFormat="1" ht="25" customHeight="1" spans="1:8">
-      <c r="A12" s="96">
+      <c r="G11" s="74"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="110"/>
+    </row>
+    <row r="12" s="59" customFormat="1" ht="25" customHeight="1" spans="1:8">
+      <c r="A12" s="76">
         <v>4</v>
       </c>
-      <c r="B12" s="97" t="s">
+      <c r="B12" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97" t="s">
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="102">
+      <c r="F12" s="82">
         <v>190.21</v>
       </c>
-      <c r="G12" s="103"/>
-      <c r="H12" s="104"/>
-    </row>
-    <row r="13" s="80" customFormat="1" ht="25" customHeight="1" spans="1:9">
-      <c r="A13" s="90"/>
-      <c r="B13" s="91" t="s">
+      <c r="G12" s="83"/>
+      <c r="H12" s="84"/>
+    </row>
+    <row r="13" s="60" customFormat="1" ht="25" customHeight="1" spans="1:9">
+      <c r="A13" s="70"/>
+      <c r="B13" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="91"/>
-      <c r="D13" s="91"/>
-      <c r="E13" s="92"/>
-      <c r="F13" s="93"/>
-      <c r="G13" s="94"/>
-      <c r="H13" s="101"/>
-      <c r="I13" s="130"/>
-    </row>
-    <row r="14" s="79" customFormat="1" ht="25" customHeight="1" spans="1:8">
-      <c r="A14" s="96"/>
-      <c r="B14" s="96"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="96"/>
-    </row>
-    <row r="15" s="80" customFormat="1" ht="25" customHeight="1" spans="1:9">
-      <c r="A15" s="90"/>
-      <c r="B15" s="105"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="101"/>
-      <c r="I15" s="130"/>
-    </row>
-    <row r="16" s="79" customFormat="1" ht="25" customHeight="1" spans="1:8">
-      <c r="A16" s="96"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="96"/>
-    </row>
-    <row r="17" s="79" customFormat="1" ht="3" customHeight="1" spans="1:8">
-      <c r="A17" s="107"/>
-      <c r="B17" s="108"/>
-      <c r="C17" s="109"/>
-      <c r="D17" s="109"/>
-      <c r="E17" s="109"/>
-      <c r="F17" s="110"/>
-      <c r="G17" s="111"/>
-      <c r="H17" s="112"/>
-    </row>
-    <row r="18" s="79" customFormat="1" ht="25" customHeight="1" spans="1:8">
-      <c r="A18" s="113" t="s">
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="110"/>
+    </row>
+    <row r="14" s="59" customFormat="1" ht="25" customHeight="1" spans="1:8">
+      <c r="A14" s="76"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="76"/>
+    </row>
+    <row r="15" s="60" customFormat="1" ht="25" customHeight="1" spans="1:9">
+      <c r="A15" s="70"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="110"/>
+    </row>
+    <row r="16" s="59" customFormat="1" ht="25" customHeight="1" spans="1:8">
+      <c r="A16" s="76"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="82"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="76"/>
+    </row>
+    <row r="17" s="59" customFormat="1" ht="3" customHeight="1" spans="1:8">
+      <c r="A17" s="87"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="91"/>
+      <c r="H17" s="92"/>
+    </row>
+    <row r="18" s="59" customFormat="1" ht="25" customHeight="1" spans="1:8">
+      <c r="A18" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="114"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="114"/>
-      <c r="G18" s="114"/>
-      <c r="H18" s="115"/>
-    </row>
-    <row r="19" s="79" customFormat="1" ht="3" customHeight="1" spans="1:8">
-      <c r="A19" s="116"/>
-      <c r="B19" s="117"/>
-      <c r="C19" s="117"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="117"/>
-      <c r="G19" s="117"/>
-      <c r="H19" s="118"/>
-    </row>
-    <row r="20" s="79" customFormat="1" ht="181" customHeight="1" spans="1:8">
-      <c r="A20" s="107"/>
-      <c r="B20" s="119"/>
-      <c r="C20" s="119"/>
-      <c r="D20" s="119"/>
-      <c r="E20" s="119"/>
-      <c r="F20" s="119"/>
-      <c r="G20" s="119"/>
-      <c r="H20" s="120"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="94"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="95"/>
+    </row>
+    <row r="19" s="59" customFormat="1" ht="3" customHeight="1" spans="1:8">
+      <c r="A19" s="96"/>
+      <c r="B19" s="97"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="97"/>
+      <c r="E19" s="97"/>
+      <c r="F19" s="97"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="98"/>
+    </row>
+    <row r="20" s="59" customFormat="1" ht="181" customHeight="1" spans="1:8">
+      <c r="A20" s="87"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="99"/>
+      <c r="E20" s="99"/>
+      <c r="F20" s="99"/>
+      <c r="G20" s="99"/>
+      <c r="H20" s="100"/>
     </row>
     <row r="21" ht="135" customHeight="1" spans="1:8">
-      <c r="A21" s="121"/>
-      <c r="B21" s="122"/>
-      <c r="C21" s="122"/>
-      <c r="D21" s="122"/>
-      <c r="E21" s="122"/>
-      <c r="F21" s="122"/>
-      <c r="G21" s="122"/>
-      <c r="H21" s="123"/>
+      <c r="A21" s="101"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="102"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="103"/>
     </row>
     <row r="22" ht="87" customHeight="1" spans="1:8">
-      <c r="A22" s="124" t="s">
+      <c r="A22" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="125"/>
-      <c r="C22" s="126"/>
-      <c r="D22" s="127"/>
-      <c r="E22" s="127"/>
-      <c r="F22" s="126"/>
-      <c r="G22" s="126"/>
-      <c r="H22" s="128"/>
+      <c r="B22" s="105"/>
+      <c r="C22" s="106"/>
+      <c r="D22" s="107"/>
+      <c r="E22" s="107"/>
+      <c r="F22" s="106"/>
+      <c r="G22" s="106"/>
+      <c r="H22" s="108"/>
     </row>
     <row r="23" ht="8" customHeight="1"/>
     <row r="24" ht="9" customHeight="1" spans="2:8">
-      <c r="B24" s="129" t="s">
+      <c r="B24" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="129"/>
-      <c r="D24" s="129"/>
-      <c r="E24" s="129"/>
-      <c r="F24" s="129"/>
-      <c r="G24" s="129"/>
-      <c r="H24" s="129"/>
+      <c r="C24" s="109"/>
+      <c r="D24" s="109"/>
+      <c r="E24" s="109"/>
+      <c r="F24" s="109"/>
+      <c r="G24" s="109"/>
+      <c r="H24" s="109"/>
     </row>
     <row r="25" ht="14" customHeight="1"/>
   </sheetData>
@@ -7708,20 +7000,20 @@
   <sheetPr/>
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6:F36"/>
+      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="27" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="9.625" style="1"/>
-    <col min="2" max="2" width="15.625" style="8" customWidth="1"/>
-    <col min="3" max="4" width="24.4083333333333" style="8" customWidth="1"/>
+    <col min="1" max="1" width="11.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="7" customWidth="1"/>
+    <col min="3" max="4" width="24.4083333333333" style="7" customWidth="1"/>
     <col min="5" max="5" width="24.4083333333333" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.4083333333333" style="52" customWidth="1"/>
-    <col min="7" max="7" width="19.2583333333333" style="11" customWidth="1"/>
+    <col min="6" max="6" width="24.4083333333333" style="27" customWidth="1"/>
+    <col min="7" max="7" width="19.2583333333333" style="28" customWidth="1"/>
     <col min="8" max="8" width="17.5" style="1" customWidth="1"/>
     <col min="9" max="10" width="9" style="1"/>
     <col min="11" max="12" width="5.625" style="1" customWidth="1"/>
@@ -7729,483 +7021,416 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="36" customHeight="1" spans="1:8">
-      <c r="A1" s="53"/>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
+      <c r="A1" s="29"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" s="2" customFormat="1" ht="40" customHeight="1" spans="1:8">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="55" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="1" ht="40" customHeight="1" spans="1:8">
-      <c r="A3" s="53"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="57">
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35">
         <v>45839</v>
       </c>
-      <c r="H3" s="58">
+      <c r="H3" s="36">
         <v>45869</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" ht="21" customHeight="1" spans="2:7">
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="25"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
     </row>
     <row r="5" s="2" customFormat="1" ht="50" customHeight="1" spans="1:8">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="66" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="64" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="67"/>
-      <c r="H5" s="68"/>
-    </row>
-    <row r="6" s="7" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A6" s="69" t="s">
+      <c r="C5" s="44"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="48"/>
+    </row>
+    <row r="6" s="6" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A6" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="50"/>
+    </row>
+    <row r="7" s="6" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="53"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="50"/>
+    </row>
+    <row r="8" s="6" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A8" s="53"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="50"/>
+    </row>
+    <row r="9" s="6" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="53"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="50"/>
+    </row>
+    <row r="10" s="6" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="53"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="50"/>
+    </row>
+    <row r="11" s="6" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="53"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="50"/>
+    </row>
+    <row r="12" s="6" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A12" s="53"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="50"/>
+    </row>
+    <row r="13" s="6" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A13" s="53"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="50"/>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="53"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="50"/>
+    </row>
+    <row r="15" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A15" s="53"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="50"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="53"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="50"/>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="53"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="50"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="53"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="50"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A19" s="53"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="50"/>
+    </row>
+    <row r="20" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A20" s="53"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="50"/>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="53"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="50"/>
+    </row>
+    <row r="22" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A22" s="53"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="50"/>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="53"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="50"/>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="53"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="50"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="53"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="50"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A26" s="53"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="50"/>
+    </row>
+    <row r="27" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A27" s="53"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="50"/>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="53"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="50"/>
+    </row>
+    <row r="29" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A29" s="53"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="50"/>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A30" s="53"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="50"/>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A31" s="53"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="53"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A32" s="53"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="50"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A33" s="53"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="50"/>
+    </row>
+    <row r="34" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A34" s="53"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="50"/>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A35" s="53"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="50"/>
+    </row>
+    <row r="36" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A36" s="53"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="50"/>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A37" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="70"/>
-    </row>
-    <row r="7" s="7" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A7" s="73"/>
-      <c r="B7" s="70" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="70"/>
-    </row>
-    <row r="8" s="7" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A8" s="73"/>
-      <c r="B8" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="70"/>
-    </row>
-    <row r="9" s="7" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A9" s="73"/>
-      <c r="B9" s="70" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="70"/>
-    </row>
-    <row r="10" s="7" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A10" s="73"/>
-      <c r="B10" s="70" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="70"/>
-    </row>
-    <row r="11" s="7" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A11" s="73"/>
-      <c r="B11" s="70" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="70"/>
-    </row>
-    <row r="12" s="7" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A12" s="73"/>
-      <c r="B12" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="70"/>
-    </row>
-    <row r="13" s="7" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A13" s="73"/>
-      <c r="B13" s="70" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="70"/>
-    </row>
-    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A14" s="73"/>
-      <c r="B14" s="70" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="70"/>
-    </row>
-    <row r="15" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A15" s="73"/>
-      <c r="B15" s="70" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="70"/>
-    </row>
-    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A16" s="73"/>
-      <c r="B16" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="70"/>
-    </row>
-    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A17" s="73"/>
-      <c r="B17" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="70"/>
-    </row>
-    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A18" s="73"/>
-      <c r="B18" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="70"/>
-    </row>
-    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A19" s="73"/>
-      <c r="B19" s="70" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="70"/>
-    </row>
-    <row r="20" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A20" s="73"/>
-      <c r="B20" s="70" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="70"/>
-    </row>
-    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A21" s="73"/>
-      <c r="B21" s="70" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="71"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="70"/>
-    </row>
-    <row r="22" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A22" s="73"/>
-      <c r="B22" s="70" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="71"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="70"/>
-    </row>
-    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A23" s="73"/>
-      <c r="B23" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="71"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="70"/>
-    </row>
-    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A24" s="73"/>
-      <c r="B24" s="70" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="71"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="70"/>
-    </row>
-    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A25" s="73"/>
-      <c r="B25" s="70" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="71"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="70"/>
-    </row>
-    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A26" s="73"/>
-      <c r="B26" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="71"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="70"/>
-    </row>
-    <row r="27" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A27" s="73"/>
-      <c r="B27" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="71"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="70"/>
-    </row>
-    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A28" s="73"/>
-      <c r="B28" s="70" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="71"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="70"/>
-    </row>
-    <row r="29" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A29" s="73"/>
-      <c r="B29" s="70" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="71"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="71"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="70"/>
-    </row>
-    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A30" s="73"/>
-      <c r="B30" s="70" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="71"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="70"/>
-    </row>
-    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A31" s="73"/>
-      <c r="B31" s="70" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="71"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="71"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="73"/>
-    </row>
-    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A32" s="73"/>
-      <c r="B32" s="70" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" s="71"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="71"/>
-      <c r="G32" s="71"/>
-      <c r="H32" s="70"/>
-    </row>
-    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A33" s="73"/>
-      <c r="B33" s="70" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" s="71"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="70"/>
-    </row>
-    <row r="34" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A34" s="73"/>
-      <c r="B34" s="70" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="71"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="70"/>
-    </row>
-    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A35" s="73"/>
-      <c r="B35" s="70" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="71"/>
-      <c r="D35" s="74"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="70"/>
-    </row>
-    <row r="36" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A36" s="73"/>
-      <c r="B36" s="70" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="71"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="71"/>
-      <c r="F36" s="71"/>
-      <c r="G36" s="71"/>
-      <c r="H36" s="70"/>
-    </row>
-    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A37" s="75" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="75"/>
-      <c r="C37" s="73">
+      <c r="B37" s="55"/>
+      <c r="C37" s="53">
         <f>SUM(C6:C36)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="73">
+      <c r="D37" s="53">
         <f>SUM(D6:D36)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="73">
+      <c r="E37" s="53">
         <f>SUM(E6:E36)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="73">
+      <c r="F37" s="53">
         <f>SUM(F6:F36)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="73">
+      <c r="G37" s="53">
         <f>SUM(G6:G36)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="75"/>
+      <c r="H37" s="53">
+        <f>SUM(H6:H36)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A38" s="76"/>
-      <c r="B38" s="76"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="76"/>
-      <c r="E38" s="77"/>
-      <c r="F38" s="77"/>
-      <c r="G38" s="78"/>
-      <c r="H38" s="76"/>
+      <c r="A38" s="56"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8215,9 +7440,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
-  <ignoredErrors>
-    <ignoredError sqref="B6:B36" numberStoredAsText="1"/>
-  </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -8225,411 +7447,418 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="27" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="19.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="12" style="9" customWidth="1"/>
-    <col min="4" max="4" width="12" style="10" customWidth="1"/>
-    <col min="5" max="7" width="12" style="11" customWidth="1"/>
-    <col min="8" max="9" width="12" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9" style="1"/>
-    <col min="12" max="13" width="5.625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="1"/>
+    <col min="2" max="2" width="19" style="7" customWidth="1"/>
+    <col min="3" max="14" width="9.875" style="8" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="36" customHeight="1" spans="1:9">
-      <c r="A1" s="12" t="s">
-        <v>56</v>
+    <row r="1" s="1" customFormat="1" ht="36" customHeight="1" spans="1:15">
+      <c r="A1" s="9" t="s">
+        <v>25</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-    </row>
-    <row r="2" s="2" customFormat="1" ht="40" customHeight="1" spans="2:9">
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
-    </row>
-    <row r="3" s="3" customFormat="1" ht="40" customHeight="1" spans="2:9">
-      <c r="B3" s="13"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
-    </row>
-    <row r="4" s="2" customFormat="1" ht="21" customHeight="1" spans="2:7">
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-    </row>
-    <row r="5" s="2" customFormat="1" ht="23" customHeight="1" spans="1:9">
-      <c r="A5" s="26" t="s">
-        <v>57</v>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+    </row>
+    <row r="2" s="2" customFormat="1" ht="40" customHeight="1" spans="2:14">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" s="3" customFormat="1" ht="40" customHeight="1" spans="2:14">
+      <c r="B3" s="10"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+    </row>
+    <row r="4" s="2" customFormat="1" ht="21" customHeight="1" spans="2:14">
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A5" s="15" t="s">
+        <v>26</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27" t="s">
-        <v>58</v>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16" t="s">
+        <v>27</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="46" t="s">
-        <v>55</v>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="25" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="6" s="4" customFormat="1" ht="36" customHeight="1" spans="1:9">
-      <c r="A6" s="26" t="s">
-        <v>59</v>
+    <row r="6" s="4" customFormat="1" ht="36" customHeight="1" spans="1:15">
+      <c r="A6" s="18" t="s">
+        <v>28</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>60</v>
+      <c r="B6" s="15" t="s">
+        <v>29</v>
       </c>
-      <c r="C6" s="27" t="s">
-        <v>61</v>
+      <c r="C6" s="18" t="s">
+        <v>30</v>
       </c>
-      <c r="D6" s="27" t="s">
-        <v>62</v>
+      <c r="D6" s="18" t="s">
+        <v>31</v>
       </c>
-      <c r="E6" s="27" t="s">
-        <v>63</v>
+      <c r="E6" s="18" t="s">
+        <v>32</v>
       </c>
-      <c r="F6" s="27" t="s">
-        <v>64</v>
+      <c r="F6" s="18" t="s">
+        <v>33</v>
       </c>
-      <c r="G6" s="27" t="s">
-        <v>65</v>
+      <c r="G6" s="18" t="s">
+        <v>34</v>
       </c>
-      <c r="H6" s="27" t="s">
-        <v>66</v>
+      <c r="H6" s="18" t="s">
+        <v>35</v>
       </c>
-      <c r="I6" s="46"/>
-    </row>
-    <row r="7" s="4" customFormat="1" ht="34" customHeight="1" spans="1:11">
-      <c r="A7" s="4" t="s">
-        <v>8</v>
+      <c r="I6" s="18" t="s">
+        <v>36</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
+      <c r="J6" s="18" t="s">
+        <v>37</v>
       </c>
-      <c r="C7" s="28">
-        <v>4190.26</v>
+      <c r="K6" s="18" t="s">
+        <v>38</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28">
-        <f>SUM(C7:H7)</f>
-        <v>4190.26</v>
+      <c r="L6" s="18" t="s">
+        <v>39</v>
       </c>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-    </row>
-    <row r="8" s="5" customFormat="1" ht="34" customHeight="1" spans="1:12">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
+      <c r="M6" s="18" t="s">
+        <v>40</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
+      <c r="N6" s="18" t="s">
+        <v>41</v>
       </c>
-      <c r="C8" s="29">
-        <v>10048.88</v>
+      <c r="O6" s="25"/>
+    </row>
+    <row r="7" s="4" customFormat="1" ht="34" customHeight="1" spans="1:15">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="26">
+        <f t="shared" ref="O7:O12" si="0">SUM(C7:N7)</f>
+        <v>0</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="28">
-        <f>SUM(C8:H8)</f>
-        <v>10048.88</v>
+    </row>
+    <row r="8" s="5" customFormat="1" ht="34" customHeight="1" spans="1:15">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-    </row>
-    <row r="9" s="4" customFormat="1" ht="34" customHeight="1" spans="1:11">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
+    </row>
+    <row r="9" s="4" customFormat="1" ht="34" customHeight="1" spans="1:15">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>11</v>
+    </row>
+    <row r="10" s="5" customFormat="1" ht="34" customHeight="1" spans="1:15">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
-      <c r="C9" s="28">
-        <v>43.25</v>
+    </row>
+    <row r="11" s="4" customFormat="1" ht="34" customHeight="1" spans="1:15">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28">
-        <f>SUM(C9:H9)</f>
-        <v>43.25</v>
+    </row>
+    <row r="12" s="5" customFormat="1" ht="34" customHeight="1" spans="1:15">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-    </row>
-    <row r="10" s="5" customFormat="1" ht="34" customHeight="1" spans="1:12">
-      <c r="A10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="29">
-        <v>190.21</v>
-      </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="28">
-        <f>SUM(C10:H10)</f>
-        <v>190.21</v>
-      </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-    </row>
-    <row r="11" s="4" customFormat="1" ht="34" customHeight="1" spans="1:9">
-      <c r="A11" s="31"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-    </row>
-    <row r="12" s="6" customFormat="1" ht="46" customHeight="1" spans="1:11">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="49"/>
-    </row>
-    <row r="13" s="4" customFormat="1" ht="34" customHeight="1" spans="1:9">
-      <c r="A13" s="35"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="50"/>
-    </row>
-    <row r="14" s="5" customFormat="1" ht="34" customHeight="1" spans="1:9">
-      <c r="A14" s="35"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="50"/>
-    </row>
-    <row r="15" s="6" customFormat="1" ht="46" customHeight="1" spans="1:10">
-      <c r="A15" s="32"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="48"/>
-    </row>
-    <row r="16" s="4" customFormat="1" ht="34" customHeight="1" spans="1:9">
-      <c r="A16" s="35"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="50"/>
-    </row>
-    <row r="17" s="5" customFormat="1" ht="34" customHeight="1" spans="1:9">
-      <c r="A17" s="35"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="50"/>
-    </row>
-    <row r="18" s="6" customFormat="1" ht="46" customHeight="1" spans="1:10">
-      <c r="A18" s="32"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="51"/>
-    </row>
-    <row r="19" s="7" customFormat="1" ht="28" customHeight="1" spans="1:9">
-      <c r="A19" s="41"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" s="7" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
-      <c r="E20" s="44"/>
-    </row>
-    <row r="21" s="7" customFormat="1" hidden="1" customHeight="1" spans="1:5">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
-      <c r="E21" s="45"/>
-    </row>
-    <row r="22" s="7" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
-      <c r="E22" s="45"/>
-    </row>
-    <row r="23" s="7" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A23" s="41"/>
-      <c r="B23" s="41"/>
-      <c r="E23" s="45"/>
-    </row>
-    <row r="24" s="7" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
-      <c r="E24" s="45"/>
-    </row>
-    <row r="25" s="7" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
-      <c r="E25" s="45"/>
-    </row>
-    <row r="26" s="7" customFormat="1" customHeight="1" spans="5:5">
-      <c r="E26" s="45"/>
-    </row>
-    <row r="27" s="7" customFormat="1" customHeight="1" spans="5:5">
-      <c r="E27" s="45"/>
-    </row>
-    <row r="28" s="7" customFormat="1" customHeight="1" spans="5:5">
-      <c r="E28" s="45"/>
-    </row>
-    <row r="29" s="7" customFormat="1" customHeight="1" spans="5:5">
-      <c r="E29" s="45"/>
-    </row>
-    <row r="30" s="7" customFormat="1" customHeight="1" spans="5:5">
-      <c r="E30" s="45"/>
-    </row>
-    <row r="31" s="7" customFormat="1" customHeight="1" spans="5:5">
-      <c r="E31" s="45"/>
-    </row>
-    <row r="32" s="7" customFormat="1" customHeight="1" spans="5:5">
-      <c r="E32" s="45"/>
-    </row>
-    <row r="33" s="7" customFormat="1" customHeight="1" spans="5:5">
-      <c r="E33" s="45"/>
-    </row>
-    <row r="34" s="7" customFormat="1" customHeight="1" spans="5:5">
-      <c r="E34" s="45"/>
-    </row>
-    <row r="35" s="7" customFormat="1" customHeight="1" spans="5:5">
-      <c r="E35" s="45"/>
-    </row>
-    <row r="36" s="7" customFormat="1" customHeight="1" spans="5:5">
-      <c r="E36" s="45"/>
-    </row>
-    <row r="37" s="1" customFormat="1" customHeight="1" spans="2:7">
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-    </row>
-    <row r="38" s="1" customFormat="1" customHeight="1" spans="2:7">
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-    </row>
-    <row r="39" s="1" customFormat="1" customHeight="1" spans="2:7">
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-    </row>
-    <row r="40" s="1" customFormat="1" customHeight="1" spans="2:7">
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-    </row>
-    <row r="41" s="1" customFormat="1" customHeight="1" spans="2:7">
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
+    </row>
+    <row r="13" s="6" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+    </row>
+    <row r="14" s="6" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+    </row>
+    <row r="15" s="6" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+    </row>
+    <row r="16" s="6" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+    </row>
+    <row r="17" s="6" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+    </row>
+    <row r="18" s="6" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+    </row>
+    <row r="19" s="6" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+    </row>
+    <row r="20" s="6" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+    </row>
+    <row r="21" s="6" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+    </row>
+    <row r="22" s="6" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+    </row>
+    <row r="23" s="6" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+    </row>
+    <row r="24" s="6" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+    </row>
+    <row r="25" s="6" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+    </row>
+    <row r="26" s="6" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
+    </row>
+    <row r="27" s="6" customFormat="1" customHeight="1"/>
+    <row r="28" s="6" customFormat="1" customHeight="1"/>
+    <row r="29" s="6" customFormat="1" customHeight="1"/>
+    <row r="30" s="6" customFormat="1" customHeight="1"/>
+    <row r="31" s="6" customFormat="1" customHeight="1"/>
+    <row r="32" s="6" customFormat="1" customHeight="1"/>
+    <row r="33" s="6" customFormat="1" customHeight="1"/>
+    <row r="34" s="6" customFormat="1" customHeight="1"/>
+    <row r="35" s="6" customFormat="1" customHeight="1"/>
+    <row r="36" s="6" customFormat="1" customHeight="1"/>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="2:14">
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="2:14">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="2:14">
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="2:14">
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+    </row>
+    <row r="41" s="1" customFormat="1" customHeight="1" spans="2:14">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="O5:O6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>